<commit_message>
Cleanup and functionality additions
</commit_message>
<xml_diff>
--- a/Assets/Resources/GameDatabase.xlsx
+++ b/Assets/Resources/GameDatabase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amyel\Documents\_Projects\Game_Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amyel\Documents\_Projects\Game_Log\GameLog\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7817A4A-2FA6-4D7B-BABB-585A0028D2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6BB6C9-7EAD-4D9B-BE42-E1EE4AB3832D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8CA71B97-9D94-4C39-8BD4-89D4608A60CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -65,9 +65,6 @@
     <t>ps2</t>
   </si>
   <si>
-    <t>completed</t>
-  </si>
-  <si>
     <t>halo</t>
   </si>
   <si>
@@ -80,10 +77,28 @@
     <t>xbox</t>
   </si>
   <si>
-    <t>library</t>
-  </si>
-  <si>
     <t>platforms</t>
+  </si>
+  <si>
+    <t>animal crossing</t>
+  </si>
+  <si>
+    <t>cute</t>
+  </si>
+  <si>
+    <t>nintendo</t>
+  </si>
+  <si>
+    <t>3ds</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>InProgress</t>
   </si>
 </sst>
 </file>
@@ -497,16 +512,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3181BEDB-80ED-4E2D-9183-89E2E0BBAEC6}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
     <col min="3" max="3" width="56.140625" customWidth="1"/>
     <col min="4" max="4" width="29.140625" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
@@ -527,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -550,7 +565,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
@@ -558,19 +573,507 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>